<commit_message>
+Attempted to handle the exception in question6 +Added some annotations
</commit_message>
<xml_diff>
--- a/Data/Output/Question6.xlsx
+++ b/Data/Output/Question6.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Shireen_Day_3\Data\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\UiPath\Shireen_Day_3_1\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDC3284-FFBE-469F-BC33-5799D4ED8CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B12AFEA-8A51-460E-A1E0-D184920E0CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="2205" yWindow="2205" windowWidth="18000" windowHeight="9360" firstSheet="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="0" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Screener" sheetId="2" r:id="rId1"/>
     <x:sheet name="Screener1" sheetId="5" r:id="rId2"/>
-    <x:sheet name="Filtered" sheetId="6" r:id="rId6"/>
+    <x:sheet name="Filtered" sheetId="6" r:id="rId3"/>
+    <x:sheet name="Screener2" sheetId="7" r:id="rId4"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="0"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <x:si>
     <x:t>INFY</x:t>
   </x:si>
@@ -137,6 +138,24 @@
   </x:si>
   <x:si>
     <x:t>₹ 36.9 / 17.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>High</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Low</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1,733</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1,305</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5.00</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -486,9 +505,9 @@
       <x:selection activeCell="A1" sqref="A1 A1:E21"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <x:sheetData>
-    <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -499,7 +518,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B2" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
@@ -510,7 +529,7 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B3" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
@@ -521,7 +540,7 @@
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B4" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
@@ -532,7 +551,7 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B5" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -543,7 +562,7 @@
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B6" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -554,7 +573,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B7" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -565,7 +584,7 @@
         <x:v>6</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B8" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -576,7 +595,7 @@
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B9" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
@@ -587,7 +606,7 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B10" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
@@ -598,7 +617,7 @@
         <x:v>9</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B11" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -609,7 +628,7 @@
         <x:v>10</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B12" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -620,7 +639,7 @@
         <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B13" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -631,7 +650,7 @@
         <x:v>12</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B14" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -642,7 +661,7 @@
         <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B15" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -653,7 +672,7 @@
         <x:v>14</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B16" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -664,7 +683,7 @@
         <x:v>15</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B17" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
@@ -675,7 +694,7 @@
         <x:v>16</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B18" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
@@ -686,7 +705,7 @@
         <x:v>17</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B19" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
@@ -697,7 +716,7 @@
         <x:v>18</x:v>
       </x:c>
     </x:row>
-    <x:row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="B20" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
@@ -722,15 +741,15 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1"/>
+  <x:dimension ref="A1:D21"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
+    <x:sheetView workbookViewId="0">
       <x:selection activeCell="D25" sqref="D25 A1:D25"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
+    <x:row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A1" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -744,7 +763,7 @@
         <x:v>23</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:4">
+    <x:row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A2" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -758,7 +777,7 @@
         <x:v>26</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:4">
+    <x:row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A3" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
@@ -772,7 +791,7 @@
         <x:v>29</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:4">
+    <x:row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A4" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
@@ -786,7 +805,7 @@
         <x:v>32</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:4">
+    <x:row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A5" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
@@ -800,7 +819,7 @@
         <x:v>29</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:4">
+    <x:row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A6" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -814,7 +833,7 @@
         <x:v>29</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:4">
+    <x:row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A7" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -828,72 +847,72 @@
         <x:v>29</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:4">
+    <x:row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A8" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:4">
+    <x:row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A9" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:4">
+    <x:row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A10" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:4">
+    <x:row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A11" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:4">
+    <x:row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A12" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:4">
+    <x:row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A13" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:4">
+    <x:row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A14" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:4">
+    <x:row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A15" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:4">
+    <x:row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A16" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:4">
+    <x:row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A17" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:4">
+    <x:row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A18" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:4">
+    <x:row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A19" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
     </x:row>
-    <x:row r="20" spans="1:4">
+    <x:row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A20" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
     </x:row>
-    <x:row r="21" spans="1:4">
+    <x:row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <x:c r="A21" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
@@ -908,7 +927,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0200-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -916,7 +935,7 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <x:sheetData/>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -924,4 +943,54 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0300-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="H10" sqref="H10 A1:H10"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:8">
+      <x:c r="A1" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:8">
+      <x:c r="A2" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>